<commit_message>
slight tweaks in the car times
</commit_message>
<xml_diff>
--- a/Data_files/Part_2/Rotterdam_car_times.xlsx
+++ b/Data_files/Part_2/Rotterdam_car_times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52922D61-CEDE-4A04-B6CE-723E475E71F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BDD361-B905-4F85-A593-7C9BF6BFF9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,13 +549,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.90625" customWidth="1"/>
+    <col min="12" max="12" width="15.36328125" customWidth="1"/>
+    <col min="13" max="13" width="14.36328125" customWidth="1"/>
+    <col min="14" max="14" width="19.7265625" customWidth="1"/>
+    <col min="15" max="15" width="18.1796875" customWidth="1"/>
+    <col min="16" max="16" width="14.6328125" customWidth="1"/>
+    <col min="23" max="23" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="51" customHeight="1" x14ac:dyDescent="0.35">
@@ -831,7 +837,7 @@
         <v>x</v>
       </c>
       <c r="M4" s="5">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N4" s="5" t="str">
         <v>x</v>
@@ -861,7 +867,7 @@
         <v>x</v>
       </c>
       <c r="W4" s="5">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="X4" s="5" t="str">
         <v>x</v>
@@ -1205,7 +1211,7 @@
         <v>22</v>
       </c>
       <c r="H9" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>22</v>
@@ -1335,7 +1341,7 @@
         <v>13</v>
       </c>
       <c r="Y10" s="5">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
@@ -1491,7 +1497,7 @@
         <v>x</v>
       </c>
       <c r="Y12" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
@@ -1985,7 +1991,7 @@
         <v>22</v>
       </c>
       <c r="H19" s="4">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>22</v>
@@ -2159,13 +2165,13 @@
         <v>22</v>
       </c>
       <c r="N21" s="9">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="O21" s="9">
         <v>11</v>
       </c>
       <c r="P21" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q21" s="9" t="s">
         <v>22</v>

</xml_diff>